<commit_message>
Added Config, added When
</commit_message>
<xml_diff>
--- a/TestingToolStable/Applications/C#Models/ProducerCSharp/ConfigTestScript.xlsx
+++ b/TestingToolStable/Applications/C#Models/ProducerCSharp/ConfigTestScript.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingToolStable\Applications\C#Models\ContractModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubPhD\rpa-testing\TestingToolStable\Applications\C#Models\ProducerCSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBCBE00-9966-4009-B78A-0E3A58A7713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5A6AAF-7988-42C1-BF68-E2628058F0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -60,19 +60,19 @@
     <t>testQueue</t>
   </si>
   <si>
-    <t>C:\Users\adelinas\AppData\Local\Programs\Python\Python38</t>
-  </si>
-  <si>
     <t>IntegrationScriptFullPath</t>
   </si>
   <si>
     <t>PythonHomePath</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingToolStable</t>
+    <t>C:\Users\marin\AppData\Local\Programs\Python\Python38</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingToolStable\integrationScript.py</t>
+    <t>C:\Users\marin\Documents\Doctorat\rpa-testing\TestingToolStable</t>
+  </si>
+  <si>
+    <t>C:\Users\marin\Documents\Doctorat\TestingToolStable\integrationScript.py</t>
   </si>
 </sst>
 </file>
@@ -459,15 +459,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="111.21875" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="111.28515625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -518,10 +518,10 @@
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -542,7 +542,7 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
@@ -1562,12 +1562,12 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1604,7 +1604,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>